<commit_message>
Add Import But Not Success
</commit_message>
<xml_diff>
--- a/exports/user(23)_transactions.xlsx
+++ b/exports/user(23)_transactions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>Transaction ID</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>ค่าเดินทาง</t>
+  </si>
+  <si>
+    <t>2024-07-02 17:17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omelet </t>
   </si>
 </sst>
 </file>
@@ -501,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
@@ -948,6 +954,35 @@
         <v>26</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>72</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16">
+        <v>500</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add ExportTemplate , Record in Import Unfinishing
</commit_message>
<xml_diff>
--- a/exports/user(23)_transactions.xlsx
+++ b/exports/user(23)_transactions.xlsx
@@ -11,12 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
+  <si>
+    <t>User Name: Kitsapas Chanlee</t>
+  </si>
+  <si>
+    <t>Created At: 2024-07-03 10:43:08</t>
+  </si>
   <si>
     <t>Transaction ID</t>
   </si>
   <si>
-    <t>Category ID</t>
+    <t>Categorie ID</t>
   </si>
   <si>
     <t>Datetime</t>
@@ -507,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I19"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
@@ -519,468 +525,478 @@
     <col min="9" max="9" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>27</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
-        <v>2000</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="I4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>2000</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>30000</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7">
-        <v>30000</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="D8">
-        <v>30000</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9">
-        <v>200</v>
+        <v>30000</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>30000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
         <v>28</v>
-      </c>
-      <c r="D10">
-        <v>120</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11">
-        <v>150.5</v>
+        <v>30000</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D12">
-        <v>300.75</v>
+        <v>200</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D13">
-        <v>100.25</v>
+        <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D14">
-        <v>100.25</v>
+        <v>150.5</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D15">
-        <v>10.25</v>
+        <v>300.75</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>41</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>100.25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>100.25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>10.25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>72</v>
       </c>
-      <c r="B16">
+      <c r="B19">
         <v>5</v>
       </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16">
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19">
         <v>500</v>
       </c>
-      <c r="E16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
-        <v>13</v>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>